<commit_message>
AIP-491 AIP-997 Variable names change and code refactoring to address review comments
Also, removed CAM_734_1 test case and combined that into CAM_734 as its
just one regression test case.
Also, Collated the test data Excel files.
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_734.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_734.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1AE53B-58C3-4A41-8881-14C3F9F05948}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25695BF6-2EA0-4E64-924C-440D45534E82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20616" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>DeviceName</t>
   </si>
@@ -58,9 +58,6 @@
     <t>PostFaultTime</t>
   </si>
   <si>
-    <t>OmicronFile</t>
-  </si>
-  <si>
     <t>MaxDFR</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>70</t>
   </si>
   <si>
-    <t>RecordDuration</t>
-  </si>
-  <si>
     <t>500</t>
   </si>
   <si>
@@ -109,10 +103,25 @@
     <t>CAM_734_1.seq</t>
   </si>
   <si>
-    <t>RecordDuration1</t>
-  </si>
-  <si>
     <t>FRSensorName1</t>
+  </si>
+  <si>
+    <t>ExpectedRecordDuration_1</t>
+  </si>
+  <si>
+    <t>ExpectedRecordDuration_2</t>
+  </si>
+  <si>
+    <t>ExpectedRecordDuration_3</t>
+  </si>
+  <si>
+    <t>ExpectedRecordDuration_4</t>
+  </si>
+  <si>
+    <t>OmicronFile_1</t>
+  </si>
+  <si>
+    <t>OmicronFile_2</t>
   </si>
 </sst>
 </file>
@@ -431,31 +440,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -481,37 +490,46 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
         <v>29</v>
       </c>
       <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
       <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" t="s">
-        <v>20</v>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -531,13 +549,13 @@
         <v>409026540</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1">
         <v>600</v>
@@ -546,28 +564,37 @@
         <v>500</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" t="s">
         <v>23</v>
       </c>
-      <c r="R2" t="s">
-        <v>24</v>
+      <c r="S2" s="1">
+        <v>600</v>
+      </c>
+      <c r="T2">
+        <v>600</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -576,7 +603,7 @@
       <c r="L3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>

</xml_diff>

<commit_message>
AIP-491 AIP-951 Updated File Name for Omicron_2.seq
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_734.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_734.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25695BF6-2EA0-4E64-924C-440D45534E82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B0F266-3AB8-492D-89DD-BB56746FBBF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>DeviceName</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>OmicronFile_2</t>
+  </si>
+  <si>
+    <t>CAM_734_2.seq</t>
   </si>
 </sst>
 </file>
@@ -442,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,12 +459,13 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -591,7 +595,7 @@
         <v>600</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>